<commit_message>
lamda new init guesses
</commit_message>
<xml_diff>
--- a/supplementary/data1/lamda.xlsx
+++ b/supplementary/data1/lamda.xlsx
@@ -767,7 +767,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -804,13 +804,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.022727994743597</v>
+        <v>6.996687583894611</v>
       </c>
       <c r="C2" t="n">
-        <v>7.001451269911716</v>
+        <v>6.976823627615556</v>
       </c>
       <c r="D2" t="n">
-        <v>7.043095782801176</v>
+        <v>7.017785375982857</v>
       </c>
       <c r="E2" t="n">
         <v>7</v>
@@ -823,13 +823,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2091616986195596</v>
+        <v>0.204292133285748</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1992228098239391</v>
+        <v>0.1936113303745512</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2187902790178325</v>
+        <v>0.2138933491786145</v>
       </c>
       <c r="E3" t="n">
         <v>0.2</v>
@@ -842,13 +842,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.05218512846532474</v>
+        <v>0.05422331215465174</v>
       </c>
       <c r="C4" t="n">
-        <v>0.045315058332322</v>
+        <v>0.0478392138545554</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0587455024411168</v>
+        <v>0.0607639377558007</v>
       </c>
       <c r="E4" t="n">
         <v>0.05</v>
@@ -857,52 +857,62 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>SNR</t>
+          <t>pi</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3.762770320018685</v>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+        <v>0.1731204375081504</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1587147316212725</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1893954936444539</v>
+      </c>
       <c r="E5" t="n">
-        <v>3.75889905491011</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>MCC</t>
+          <t>Keq</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9914311130105118</v>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+        <v>0.2104955595729849</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.1886574486983213</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.2336472656222764</v>
+      </c>
       <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Recall</t>
+          <t>SNR</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.9976076555023924</v>
+        <v>3.761977261134855</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>3.75889905491011</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Precision</t>
+          <t>MCC</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9881516587677726</v>
+        <v>0.9914675955572496</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
@@ -911,11 +921,11 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>Recall</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2077</v>
+        <v>1</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -924,11 +934,11 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>Precision</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>5</v>
+        <v>0.9858490566037735</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -937,11 +947,11 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>2076</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -950,11 +960,11 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>417</v>
+        <v>6</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -963,32 +973,45 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>p(specific)</t>
+          <t>FN</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.9993148753524894</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.9984820107113446</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.999534151404019</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>pi</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>418</v>
+      </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="n">
-        <v>0.15</v>
-      </c>
+      <c r="E14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>p(specific)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.9993281923871153</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.9985745993077032</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.9995282850021244</v>
+      </c>
+      <c r="E15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1001,7 +1024,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1038,13 +1061,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.059353007254505</v>
+        <v>7.091339770682374</v>
       </c>
       <c r="C2" t="n">
-        <v>7.041127258934724</v>
+        <v>7.070818935122439</v>
       </c>
       <c r="D2" t="n">
-        <v>7.078867813755407</v>
+        <v>7.113135877405636</v>
       </c>
       <c r="E2" t="n">
         <v>7</v>
@@ -1057,13 +1080,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2238280556075518</v>
+        <v>0.2171760650968842</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2125133761071408</v>
+        <v>0.2053141933922834</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2371278567395072</v>
+        <v>0.2278114621634793</v>
       </c>
       <c r="E3" t="n">
         <v>0.2</v>
@@ -1076,13 +1099,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9649731836397113</v>
+        <v>0.9913055644816908</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9379540409381856</v>
+        <v>0.9630704462345296</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9919528243421496</v>
+        <v>1.018960305113115</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
@@ -1091,52 +1114,62 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>SNR</t>
+          <t>pi</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3.854975487441888</v>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+        <v>0.1737028249976817</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1592361811506343</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1900410159483033</v>
+      </c>
       <c r="E5" t="n">
-        <v>3.75889905491011</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>MCC</t>
+          <t>Keq</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9141383758314683</v>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+        <v>0.2113543413197227</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.1893946654237603</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.2346304610812667</v>
+      </c>
       <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Recall</t>
+          <t>SNR</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.9090909090909091</v>
+        <v>3.948417826326017</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>3.75889905491011</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Precision</t>
+          <t>MCC</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9476309226932669</v>
+        <v>0.9622567739333436</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
@@ -1145,11 +1178,11 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>Recall</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2061</v>
+        <v>0.9904306220095693</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -1158,11 +1191,11 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>Precision</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>21</v>
+        <v>0.9473684210526315</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -1171,11 +1204,11 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>38</v>
+        <v>2059</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -1184,11 +1217,11 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>380</v>
+        <v>23</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -1197,32 +1230,45 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>p(specific)</t>
+          <t>FN</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.9850866426576983</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.9506766137932414</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.9922806231006812</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>pi</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>414</v>
+      </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="n">
-        <v>0.15</v>
-      </c>
+      <c r="E14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>p(specific)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.9885547964978505</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.975139958193761</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.9940717758244612</v>
+      </c>
+      <c r="E15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1235,7 +1281,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1272,13 +1318,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.018226275604579</v>
+        <v>7.006089850771027</v>
       </c>
       <c r="C2" t="n">
-        <v>6.998955784334632</v>
+        <v>6.985053242317973</v>
       </c>
       <c r="D2" t="n">
-        <v>7.039493613220144</v>
+        <v>7.028435075021673</v>
       </c>
       <c r="E2" t="n">
         <v>7</v>
@@ -1291,13 +1337,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2075977684355938</v>
+        <v>0.2027042158313969</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1989136331247141</v>
+        <v>0.192454572273346</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2171932863770461</v>
+        <v>0.2119043999479361</v>
       </c>
       <c r="E3" t="n">
         <v>0.2</v>
@@ -1310,13 +1356,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.01049713921090711</v>
+        <v>0.01039546471149803</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0078626135056757</v>
+        <v>0.007691950981008</v>
       </c>
       <c r="D4" t="n">
-        <v>0.01335417569</v>
+        <v>0.0133870759672566</v>
       </c>
       <c r="E4" t="n">
         <v>0.01</v>
@@ -1325,52 +1371,62 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>SNR</t>
+          <t>pi</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3.756197420760612</v>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+        <v>0.1732564768707913</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1584778611899527</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1899691401107213</v>
+      </c>
       <c r="E5" t="n">
-        <v>3.75889905491011</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>MCC</t>
+          <t>Keq</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9971369288120798</v>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+        <v>0.2107273659127262</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.1883228670989748</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.234520911207085</v>
+      </c>
       <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Recall</t>
+          <t>SNR</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>3.749766130642911</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>3.75889905491011</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Precision</t>
+          <t>MCC</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9952380952380953</v>
+        <v>0.9985660739664485</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
@@ -1379,11 +1435,11 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>Recall</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2080</v>
+        <v>1</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -1392,11 +1448,11 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>Precision</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>0.9976133651551312</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -1405,11 +1461,11 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>2081</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -1418,11 +1474,11 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>418</v>
+        <v>1</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -1431,32 +1487,45 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>p(specific)</t>
+          <t>FN</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.9998637185716288</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.9997030657292124</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.999908072642169</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>pi</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>418</v>
+      </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="n">
-        <v>0.15</v>
-      </c>
+      <c r="E14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>p(specific)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.9998729624295279</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.9997184600760852</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.9999131081282366</v>
+      </c>
+      <c r="E15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1469,7 +1538,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1506,13 +1575,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.02809494081569</v>
+        <v>7.093184567093628</v>
       </c>
       <c r="C2" t="n">
-        <v>7.010201828321613</v>
+        <v>7.07258619372312</v>
       </c>
       <c r="D2" t="n">
-        <v>7.046437121665874</v>
+        <v>7.115063148529826</v>
       </c>
       <c r="E2" t="n">
         <v>7</v>
@@ -1525,13 +1594,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2248685577803758</v>
+        <v>0.2152565921174508</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2117913302976286</v>
+        <v>0.2032320271264699</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2378276717772655</v>
+        <v>0.2260526857329364</v>
       </c>
       <c r="E3" t="n">
         <v>0.2</v>
@@ -1544,13 +1613,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.4963091859866898</v>
+        <v>0.4914945559425632</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4791702353991057</v>
+        <v>0.4733921863139085</v>
       </c>
       <c r="D4" t="n">
-        <v>0.516827345833419</v>
+        <v>0.5092979513473626</v>
       </c>
       <c r="E4" t="n">
         <v>0.5</v>
@@ -1559,52 +1628,62 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>SNR</t>
+          <t>pi</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3.832522909637779</v>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+        <v>0.1732984386545297</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1587799969581947</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1897036573362159</v>
+      </c>
       <c r="E5" t="n">
-        <v>3.75889905491011</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>MCC</t>
+          <t>Keq</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9453189697761857</v>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+        <v>0.210766110079728</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.188749669744199</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.2341164349915773</v>
+      </c>
       <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Recall</t>
+          <t>SNR</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.9521531100478469</v>
+        <v>3.843139606860399</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>3.75889905491011</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Precision</t>
+          <t>MCC</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9567307692307693</v>
+        <v>0.971955289238697</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
@@ -1613,11 +1692,11 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>Recall</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2064</v>
+        <v>0.9952153110047847</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -1626,11 +1705,11 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>Precision</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>18</v>
+        <v>0.9585253456221198</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -1639,11 +1718,11 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>20</v>
+        <v>2064</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -1652,11 +1731,11 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>398</v>
+        <v>18</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -1665,32 +1744,45 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>p(specific)</t>
+          <t>FN</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.9925934429726241</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.9814218766839864</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.9958672803299444</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>pi</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>416</v>
+      </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="n">
-        <v>0.15</v>
-      </c>
+      <c r="E14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>p(specific)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.9940361218491627</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.9870758688439624</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.997106970967898</v>
+      </c>
+      <c r="E15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1703,7 +1795,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1740,13 +1832,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.005398985677058</v>
+        <v>7.002403255994217</v>
       </c>
       <c r="C2" t="n">
-        <v>6.986706843924773</v>
+        <v>6.981462514546145</v>
       </c>
       <c r="D2" t="n">
-        <v>7.025882512786813</v>
+        <v>7.02464650658167</v>
       </c>
       <c r="E2" t="n">
         <v>7</v>
@@ -1759,13 +1851,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2161735921165374</v>
+        <v>0.2082011137697973</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2065305238086126</v>
+        <v>0.1980091052580437</v>
       </c>
       <c r="D3" t="n">
-        <v>0.225501462342905</v>
+        <v>0.217351398503064</v>
       </c>
       <c r="E3" t="n">
         <v>0.2</v>
@@ -1778,13 +1870,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1577208517393283</v>
+        <v>0.1542698026731528</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1484949816689978</v>
+        <v>0.1433309674317986</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1686415800836434</v>
+        <v>0.1652123308767115</v>
       </c>
       <c r="E4" t="n">
         <v>0.15</v>
@@ -1793,52 +1885,62 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>SNR</t>
+          <t>pi</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3.777836589444367</v>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+        <v>0.172155532464627</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1584130878392987</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1876643266692657</v>
+      </c>
       <c r="E5" t="n">
-        <v>3.75889905491011</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>MCC</t>
+          <t>Keq</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9799840914864164</v>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+        <v>0.2090268040384629</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.1882314066731731</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.2310182362033923</v>
+      </c>
       <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Recall</t>
+          <t>SNR</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.9880382775119617</v>
+        <v>3.787464886780817</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>3.75889905491011</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Precision</t>
+          <t>MCC</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9786729857819905</v>
+        <v>0.9872644337931913</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
@@ -1847,11 +1949,11 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>Recall</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2073</v>
+        <v>1</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -1860,11 +1962,11 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>Precision</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>9</v>
+        <v>0.9789227166276346</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -1873,11 +1975,11 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>5</v>
+        <v>2073</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -1886,11 +1988,11 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>413</v>
+        <v>9</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -1899,32 +2001,45 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>p(specific)</t>
+          <t>FN</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.9977434587537986</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.9950877359825548</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.9984371402340294</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>pi</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>418</v>
+      </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="n">
-        <v>0.15</v>
-      </c>
+      <c r="E14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>p(specific)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.9980787137566742</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.9959616337693512</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.9986518429881251</v>
+      </c>
+      <c r="E15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>